<commit_message>
fixed layouts and plot resoulitons
</commit_message>
<xml_diff>
--- a/psychDiagnosis/excel/PCLRWords.xlsx
+++ b/psychDiagnosis/excel/PCLRWords.xlsx
@@ -503,7 +503,7 @@
       </c>
       <c r="C2" s="6" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Very Glib</t>
         </is>
       </c>
       <c r="E2" s="4" t="inlineStr">
@@ -525,7 +525,7 @@
       </c>
       <c r="C3" s="6" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Very Grandiose</t>
         </is>
       </c>
       <c r="E3" s="4" t="inlineStr">
@@ -547,7 +547,7 @@
       </c>
       <c r="C4" s="6" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Very Conniving</t>
         </is>
       </c>
       <c r="E4" s="4" t="inlineStr">
@@ -569,7 +569,7 @@
       </c>
       <c r="C5" s="6" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Very Deceptive</t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
@@ -591,7 +591,7 @@
       </c>
       <c r="C6" s="6" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Very Unremorseful</t>
         </is>
       </c>
       <c r="E6" s="4" t="inlineStr">
@@ -613,7 +613,7 @@
       </c>
       <c r="C7" s="6" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Very Callous</t>
         </is>
       </c>
       <c r="E7" s="4" t="inlineStr">
@@ -635,7 +635,7 @@
       </c>
       <c r="C8" s="6" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Very Inexpressive</t>
         </is>
       </c>
       <c r="E8" s="4" t="inlineStr">
@@ -657,7 +657,7 @@
       </c>
       <c r="C9" s="6" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Very Irresponsible</t>
         </is>
       </c>
       <c r="E9" s="4" t="inlineStr">
@@ -679,7 +679,7 @@
       </c>
       <c r="C10" s="6" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Very Sensation Seeking</t>
         </is>
       </c>
       <c r="E10" s="4" t="inlineStr">
@@ -701,7 +701,7 @@
       </c>
       <c r="C11" s="6" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Very Unrealistic</t>
         </is>
       </c>
       <c r="E11" s="4" t="inlineStr">
@@ -723,7 +723,7 @@
       </c>
       <c r="C12" s="6" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Very Impulsive</t>
         </is>
       </c>
       <c r="E12" s="4" t="inlineStr">
@@ -745,7 +745,7 @@
       </c>
       <c r="C13" s="6" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Very Irresponsible</t>
         </is>
       </c>
       <c r="E13" s="4" t="inlineStr">
@@ -767,7 +767,7 @@
       </c>
       <c r="C14" s="6" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Very Parasitic</t>
         </is>
       </c>
       <c r="E14" s="4" t="inlineStr">
@@ -789,7 +789,7 @@
       </c>
       <c r="C15" s="6" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Very Noncommittal</t>
         </is>
       </c>
       <c r="E15" s="4" t="inlineStr">
@@ -811,7 +811,7 @@
       </c>
       <c r="C16" s="6" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Very Promiscuous</t>
         </is>
       </c>
       <c r="E16" s="4" t="inlineStr">
@@ -833,7 +833,7 @@
       </c>
       <c r="C17" s="6" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Very Emotionally Controlled</t>
         </is>
       </c>
       <c r="E17" s="4" t="inlineStr">
@@ -855,7 +855,7 @@
       </c>
       <c r="C18" s="6" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Very Problematic</t>
         </is>
       </c>
       <c r="E18" s="4" t="inlineStr">
@@ -877,7 +877,7 @@
       </c>
       <c r="C19" s="6" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Very Delinquent</t>
         </is>
       </c>
       <c r="E19" s="4" t="inlineStr">
@@ -899,7 +899,7 @@
       </c>
       <c r="C20" s="6" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Very Noncompliant</t>
         </is>
       </c>
       <c r="E20" s="4" t="inlineStr">
@@ -921,7 +921,7 @@
       </c>
       <c r="C21" s="6" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Very Versatile</t>
         </is>
       </c>
       <c r="E21" s="4" t="inlineStr">

</xml_diff>

<commit_message>
Fixed plotting issues and trees
</commit_message>
<xml_diff>
--- a/psychDiagnosis/excel/PCLRWords.xlsx
+++ b/psychDiagnosis/excel/PCLRWords.xlsx
@@ -503,7 +503,7 @@
       </c>
       <c r="C2" s="6" t="inlineStr">
         <is>
-          <t>Very Glib</t>
+          <t>Fairly Glib</t>
         </is>
       </c>
       <c r="E2" s="4" t="inlineStr">
@@ -525,7 +525,7 @@
       </c>
       <c r="C3" s="6" t="inlineStr">
         <is>
-          <t>Very Grandiose</t>
+          <t>Fairly Grandiose</t>
         </is>
       </c>
       <c r="E3" s="4" t="inlineStr">
@@ -547,7 +547,7 @@
       </c>
       <c r="C4" s="6" t="inlineStr">
         <is>
-          <t>Very Conniving</t>
+          <t>Fairly Conniving</t>
         </is>
       </c>
       <c r="E4" s="4" t="inlineStr">
@@ -569,7 +569,7 @@
       </c>
       <c r="C5" s="6" t="inlineStr">
         <is>
-          <t>Very Deceptive</t>
+          <t>Fairly Deceptive</t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
@@ -591,7 +591,7 @@
       </c>
       <c r="C6" s="6" t="inlineStr">
         <is>
-          <t>Very Unremorseful</t>
+          <t>Fairly Unremorseful</t>
         </is>
       </c>
       <c r="E6" s="4" t="inlineStr">
@@ -613,7 +613,7 @@
       </c>
       <c r="C7" s="6" t="inlineStr">
         <is>
-          <t>Very Callous</t>
+          <t>Fairly Callous</t>
         </is>
       </c>
       <c r="E7" s="4" t="inlineStr">
@@ -635,7 +635,7 @@
       </c>
       <c r="C8" s="6" t="inlineStr">
         <is>
-          <t>Very Inexpressive</t>
+          <t>Fairly Inexpressive</t>
         </is>
       </c>
       <c r="E8" s="4" t="inlineStr">
@@ -657,7 +657,7 @@
       </c>
       <c r="C9" s="6" t="inlineStr">
         <is>
-          <t>Very Irresponsible</t>
+          <t>Fairly Irresponsible</t>
         </is>
       </c>
       <c r="E9" s="4" t="inlineStr">
@@ -679,7 +679,7 @@
       </c>
       <c r="C10" s="6" t="inlineStr">
         <is>
-          <t>Very Sensation Seeking</t>
+          <t>Fairly Sensation Seeking</t>
         </is>
       </c>
       <c r="E10" s="4" t="inlineStr">
@@ -701,7 +701,7 @@
       </c>
       <c r="C11" s="6" t="inlineStr">
         <is>
-          <t>Very Unrealistic</t>
+          <t>Fairly Unrealistic</t>
         </is>
       </c>
       <c r="E11" s="4" t="inlineStr">
@@ -723,7 +723,7 @@
       </c>
       <c r="C12" s="6" t="inlineStr">
         <is>
-          <t>Very Impulsive</t>
+          <t>Fairly Impulsive</t>
         </is>
       </c>
       <c r="E12" s="4" t="inlineStr">
@@ -745,7 +745,7 @@
       </c>
       <c r="C13" s="6" t="inlineStr">
         <is>
-          <t>Very Irresponsible</t>
+          <t>Fairly Irresponsible</t>
         </is>
       </c>
       <c r="E13" s="4" t="inlineStr">
@@ -767,7 +767,7 @@
       </c>
       <c r="C14" s="6" t="inlineStr">
         <is>
-          <t>Very Parasitic</t>
+          <t>Fairly Parasitic</t>
         </is>
       </c>
       <c r="E14" s="4" t="inlineStr">
@@ -789,7 +789,7 @@
       </c>
       <c r="C15" s="6" t="inlineStr">
         <is>
-          <t>Very Noncommittal</t>
+          <t>Fairly Noncommittal</t>
         </is>
       </c>
       <c r="E15" s="4" t="inlineStr">
@@ -811,7 +811,7 @@
       </c>
       <c r="C16" s="6" t="inlineStr">
         <is>
-          <t>Very Promiscuous</t>
+          <t>Fairly Promiscuous</t>
         </is>
       </c>
       <c r="E16" s="4" t="inlineStr">
@@ -833,7 +833,7 @@
       </c>
       <c r="C17" s="6" t="inlineStr">
         <is>
-          <t>Very Emotionally Controlled</t>
+          <t>Fairly Emotionally Controlled</t>
         </is>
       </c>
       <c r="E17" s="4" t="inlineStr">
@@ -855,7 +855,7 @@
       </c>
       <c r="C18" s="6" t="inlineStr">
         <is>
-          <t>Very Problematic</t>
+          <t>Fairly Problematic</t>
         </is>
       </c>
       <c r="E18" s="4" t="inlineStr">
@@ -877,7 +877,7 @@
       </c>
       <c r="C19" s="6" t="inlineStr">
         <is>
-          <t>Very Delinquent</t>
+          <t>Fairly Delinquent</t>
         </is>
       </c>
       <c r="E19" s="4" t="inlineStr">
@@ -899,7 +899,7 @@
       </c>
       <c r="C20" s="6" t="inlineStr">
         <is>
-          <t>Very Noncompliant</t>
+          <t>Fairly Noncompliant</t>
         </is>
       </c>
       <c r="E20" s="4" t="inlineStr">
@@ -921,7 +921,7 @@
       </c>
       <c r="C21" s="6" t="inlineStr">
         <is>
-          <t>Very Versatile</t>
+          <t>Fairly Versatile</t>
         </is>
       </c>
       <c r="E21" s="4" t="inlineStr">

</xml_diff>

<commit_message>
Fixed issues with umf under lmf, added plots to .gitignore
</commit_message>
<xml_diff>
--- a/psychDiagnosis/excel/PCLRWords.xlsx
+++ b/psychDiagnosis/excel/PCLRWords.xlsx
@@ -503,7 +503,7 @@
       </c>
       <c r="C2" s="6" t="inlineStr">
         <is>
-          <t>Fairly Glib</t>
+          <t>Mildly Glib</t>
         </is>
       </c>
       <c r="E2" s="4" t="inlineStr">
@@ -525,7 +525,7 @@
       </c>
       <c r="C3" s="6" t="inlineStr">
         <is>
-          <t>Fairly Grandiose</t>
+          <t>Mildly Grandiose</t>
         </is>
       </c>
       <c r="E3" s="4" t="inlineStr">
@@ -547,7 +547,7 @@
       </c>
       <c r="C4" s="6" t="inlineStr">
         <is>
-          <t>Fairly Conniving</t>
+          <t>Mildly Conniving</t>
         </is>
       </c>
       <c r="E4" s="4" t="inlineStr">
@@ -569,7 +569,7 @@
       </c>
       <c r="C5" s="6" t="inlineStr">
         <is>
-          <t>Fairly Deceptive</t>
+          <t>Mildly Deceptive</t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
@@ -591,7 +591,7 @@
       </c>
       <c r="C6" s="6" t="inlineStr">
         <is>
-          <t>Fairly Unremorseful</t>
+          <t>Mildly Unremorseful</t>
         </is>
       </c>
       <c r="E6" s="4" t="inlineStr">
@@ -613,7 +613,7 @@
       </c>
       <c r="C7" s="6" t="inlineStr">
         <is>
-          <t>Fairly Callous</t>
+          <t>Mildly Callous</t>
         </is>
       </c>
       <c r="E7" s="4" t="inlineStr">
@@ -635,7 +635,7 @@
       </c>
       <c r="C8" s="6" t="inlineStr">
         <is>
-          <t>Fairly Inexpressive</t>
+          <t>Mildly Inexpressive</t>
         </is>
       </c>
       <c r="E8" s="4" t="inlineStr">
@@ -657,7 +657,7 @@
       </c>
       <c r="C9" s="6" t="inlineStr">
         <is>
-          <t>Fairly Irresponsible</t>
+          <t>Mildly Irresponsible</t>
         </is>
       </c>
       <c r="E9" s="4" t="inlineStr">
@@ -679,7 +679,7 @@
       </c>
       <c r="C10" s="6" t="inlineStr">
         <is>
-          <t>Fairly Sensation Seeking</t>
+          <t>Mildly Sensation Seeking</t>
         </is>
       </c>
       <c r="E10" s="4" t="inlineStr">
@@ -701,7 +701,7 @@
       </c>
       <c r="C11" s="6" t="inlineStr">
         <is>
-          <t>Fairly Unrealistic</t>
+          <t>Mildly Unrealistic</t>
         </is>
       </c>
       <c r="E11" s="4" t="inlineStr">
@@ -723,7 +723,7 @@
       </c>
       <c r="C12" s="6" t="inlineStr">
         <is>
-          <t>Fairly Impulsive</t>
+          <t>Mildly Impulsive</t>
         </is>
       </c>
       <c r="E12" s="4" t="inlineStr">
@@ -745,7 +745,7 @@
       </c>
       <c r="C13" s="6" t="inlineStr">
         <is>
-          <t>Fairly Irresponsible</t>
+          <t>Mildly Irresponsible</t>
         </is>
       </c>
       <c r="E13" s="4" t="inlineStr">
@@ -767,7 +767,7 @@
       </c>
       <c r="C14" s="6" t="inlineStr">
         <is>
-          <t>Fairly Parasitic</t>
+          <t>Mildly Parasitic</t>
         </is>
       </c>
       <c r="E14" s="4" t="inlineStr">
@@ -789,7 +789,7 @@
       </c>
       <c r="C15" s="6" t="inlineStr">
         <is>
-          <t>Fairly Noncommittal</t>
+          <t>Mildly Noncommittal</t>
         </is>
       </c>
       <c r="E15" s="4" t="inlineStr">
@@ -811,7 +811,7 @@
       </c>
       <c r="C16" s="6" t="inlineStr">
         <is>
-          <t>Fairly Promiscuous</t>
+          <t>Mildly Promiscuous</t>
         </is>
       </c>
       <c r="E16" s="4" t="inlineStr">
@@ -833,7 +833,7 @@
       </c>
       <c r="C17" s="6" t="inlineStr">
         <is>
-          <t>Fairly Emotionally Controlled</t>
+          <t>Mildly Emotionally Controlled</t>
         </is>
       </c>
       <c r="E17" s="4" t="inlineStr">
@@ -855,7 +855,7 @@
       </c>
       <c r="C18" s="6" t="inlineStr">
         <is>
-          <t>Fairly Problematic</t>
+          <t>Mildly Problematic</t>
         </is>
       </c>
       <c r="E18" s="4" t="inlineStr">
@@ -877,7 +877,7 @@
       </c>
       <c r="C19" s="6" t="inlineStr">
         <is>
-          <t>Fairly Delinquent</t>
+          <t>Mildly Delinquent</t>
         </is>
       </c>
       <c r="E19" s="4" t="inlineStr">
@@ -899,7 +899,7 @@
       </c>
       <c r="C20" s="6" t="inlineStr">
         <is>
-          <t>Fairly Noncompliant</t>
+          <t>Mildly Noncompliant</t>
         </is>
       </c>
       <c r="E20" s="4" t="inlineStr">
@@ -921,7 +921,7 @@
       </c>
       <c r="C21" s="6" t="inlineStr">
         <is>
-          <t>Fairly Versatile</t>
+          <t>Mildly Versatile</t>
         </is>
       </c>
       <c r="E21" s="4" t="inlineStr">

</xml_diff>

<commit_message>
Did some stuff for app
</commit_message>
<xml_diff>
--- a/psychDiagnosis/excel/PCLRWords.xlsx
+++ b/psychDiagnosis/excel/PCLRWords.xlsx
@@ -503,7 +503,7 @@
       </c>
       <c r="C2" s="6" t="inlineStr">
         <is>
-          <t>Mildly Glib</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E2" s="4" t="inlineStr">
@@ -525,7 +525,7 @@
       </c>
       <c r="C3" s="6" t="inlineStr">
         <is>
-          <t>Mildly Grandiose</t>
+          <t>Very Grandiose</t>
         </is>
       </c>
       <c r="E3" s="4" t="inlineStr">
@@ -547,7 +547,7 @@
       </c>
       <c r="C4" s="6" t="inlineStr">
         <is>
-          <t>Mildly Conniving</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E4" s="4" t="inlineStr">
@@ -569,7 +569,7 @@
       </c>
       <c r="C5" s="6" t="inlineStr">
         <is>
-          <t>Mildly Deceptive</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
@@ -591,7 +591,7 @@
       </c>
       <c r="C6" s="6" t="inlineStr">
         <is>
-          <t>Mildly Unremorseful</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E6" s="4" t="inlineStr">
@@ -613,7 +613,7 @@
       </c>
       <c r="C7" s="6" t="inlineStr">
         <is>
-          <t>Mildly Callous</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E7" s="4" t="inlineStr">
@@ -635,7 +635,7 @@
       </c>
       <c r="C8" s="6" t="inlineStr">
         <is>
-          <t>Mildly Inexpressive</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E8" s="4" t="inlineStr">
@@ -657,7 +657,7 @@
       </c>
       <c r="C9" s="6" t="inlineStr">
         <is>
-          <t>Mildly Irresponsible</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E9" s="4" t="inlineStr">
@@ -679,7 +679,7 @@
       </c>
       <c r="C10" s="6" t="inlineStr">
         <is>
-          <t>Mildly Sensation Seeking</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E10" s="4" t="inlineStr">
@@ -701,7 +701,7 @@
       </c>
       <c r="C11" s="6" t="inlineStr">
         <is>
-          <t>Mildly Unrealistic</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E11" s="4" t="inlineStr">
@@ -723,7 +723,7 @@
       </c>
       <c r="C12" s="6" t="inlineStr">
         <is>
-          <t>Mildly Impulsive</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E12" s="4" t="inlineStr">
@@ -745,7 +745,7 @@
       </c>
       <c r="C13" s="6" t="inlineStr">
         <is>
-          <t>Mildly Irresponsible</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E13" s="4" t="inlineStr">
@@ -767,7 +767,7 @@
       </c>
       <c r="C14" s="6" t="inlineStr">
         <is>
-          <t>Mildly Parasitic</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E14" s="4" t="inlineStr">
@@ -789,7 +789,7 @@
       </c>
       <c r="C15" s="6" t="inlineStr">
         <is>
-          <t>Mildly Noncommittal</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E15" s="4" t="inlineStr">
@@ -811,7 +811,7 @@
       </c>
       <c r="C16" s="6" t="inlineStr">
         <is>
-          <t>Mildly Promiscuous</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E16" s="4" t="inlineStr">
@@ -833,7 +833,7 @@
       </c>
       <c r="C17" s="6" t="inlineStr">
         <is>
-          <t>Mildly Emotionally Controlled</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E17" s="4" t="inlineStr">
@@ -855,7 +855,7 @@
       </c>
       <c r="C18" s="6" t="inlineStr">
         <is>
-          <t>Mildly Problematic</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E18" s="4" t="inlineStr">
@@ -877,7 +877,7 @@
       </c>
       <c r="C19" s="6" t="inlineStr">
         <is>
-          <t>Mildly Delinquent</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E19" s="4" t="inlineStr">
@@ -899,7 +899,7 @@
       </c>
       <c r="C20" s="6" t="inlineStr">
         <is>
-          <t>Mildly Noncompliant</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="E20" s="4" t="inlineStr">

</xml_diff>

<commit_message>
Created build script and organized project so that it can build properly
</commit_message>
<xml_diff>
--- a/psychDiagnosis/excel/PCLRWords.xlsx
+++ b/psychDiagnosis/excel/PCLRWords.xlsx
@@ -503,7 +503,7 @@
       </c>
       <c r="C2" s="6" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Mildly Glib</t>
         </is>
       </c>
       <c r="E2" s="4" t="inlineStr">
@@ -525,7 +525,7 @@
       </c>
       <c r="C3" s="6" t="inlineStr">
         <is>
-          <t>Very Grandiose</t>
+          <t>Mildly Grandiose</t>
         </is>
       </c>
       <c r="E3" s="4" t="inlineStr">
@@ -547,7 +547,7 @@
       </c>
       <c r="C4" s="6" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Mildly Conniving</t>
         </is>
       </c>
       <c r="E4" s="4" t="inlineStr">
@@ -569,7 +569,7 @@
       </c>
       <c r="C5" s="6" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Mildly Deceptive</t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
@@ -591,7 +591,7 @@
       </c>
       <c r="C6" s="6" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Mildly Unremorseful</t>
         </is>
       </c>
       <c r="E6" s="4" t="inlineStr">
@@ -613,7 +613,7 @@
       </c>
       <c r="C7" s="6" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Mildly Callous</t>
         </is>
       </c>
       <c r="E7" s="4" t="inlineStr">
@@ -635,7 +635,7 @@
       </c>
       <c r="C8" s="6" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Mildly Inexpressive</t>
         </is>
       </c>
       <c r="E8" s="4" t="inlineStr">
@@ -657,7 +657,7 @@
       </c>
       <c r="C9" s="6" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Mildly Irresponsible</t>
         </is>
       </c>
       <c r="E9" s="4" t="inlineStr">
@@ -679,7 +679,7 @@
       </c>
       <c r="C10" s="6" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Mildly Sensation Seeking</t>
         </is>
       </c>
       <c r="E10" s="4" t="inlineStr">
@@ -701,7 +701,7 @@
       </c>
       <c r="C11" s="6" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Mildly Unrealistic</t>
         </is>
       </c>
       <c r="E11" s="4" t="inlineStr">
@@ -723,7 +723,7 @@
       </c>
       <c r="C12" s="6" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Mildly Impulsive</t>
         </is>
       </c>
       <c r="E12" s="4" t="inlineStr">
@@ -745,7 +745,7 @@
       </c>
       <c r="C13" s="6" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Mildly Irresponsible</t>
         </is>
       </c>
       <c r="E13" s="4" t="inlineStr">
@@ -767,7 +767,7 @@
       </c>
       <c r="C14" s="6" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Mildly Parasitic</t>
         </is>
       </c>
       <c r="E14" s="4" t="inlineStr">
@@ -789,7 +789,7 @@
       </c>
       <c r="C15" s="6" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Mildly Noncommittal</t>
         </is>
       </c>
       <c r="E15" s="4" t="inlineStr">
@@ -811,7 +811,7 @@
       </c>
       <c r="C16" s="6" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Mildly Promiscuous</t>
         </is>
       </c>
       <c r="E16" s="4" t="inlineStr">
@@ -833,7 +833,7 @@
       </c>
       <c r="C17" s="6" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Mildly Emotionally Controlled</t>
         </is>
       </c>
       <c r="E17" s="4" t="inlineStr">
@@ -855,7 +855,7 @@
       </c>
       <c r="C18" s="6" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Mildly Problematic</t>
         </is>
       </c>
       <c r="E18" s="4" t="inlineStr">
@@ -877,7 +877,7 @@
       </c>
       <c r="C19" s="6" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Mildly Delinquent</t>
         </is>
       </c>
       <c r="E19" s="4" t="inlineStr">
@@ -899,7 +899,7 @@
       </c>
       <c r="C20" s="6" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Mildly Noncompliant</t>
         </is>
       </c>
       <c r="E20" s="4" t="inlineStr">

</xml_diff>